<commit_message>
Dtr-fgt-shoes update User& Time
</commit_message>
<xml_diff>
--- a/DKS-API/Resources/Template/TempDtrFgtEtd.xlsx
+++ b/DKS-API/Resources/Template/TempDtrFgtEtd.xlsx
@@ -56,10 +56,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>QC ETD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Remark</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -93,6 +89,10 @@
   </si>
   <si>
     <t>Update Time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QC Result Date</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -501,7 +501,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -510,8 +510,8 @@
     <col min="2" max="2" width="10.25" style="3" customWidth="1"/>
     <col min="3" max="3" width="11.25" style="3" customWidth="1"/>
     <col min="4" max="4" width="12.125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.875" style="9" customWidth="1"/>
-    <col min="6" max="6" width="15.625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="19.125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="17.375" style="10" customWidth="1"/>
     <col min="7" max="7" width="46.875" style="3" customWidth="1"/>
     <col min="8" max="8" width="14.75" style="3" customWidth="1"/>
     <col min="9" max="9" width="14.625" style="5" customWidth="1"/>
@@ -535,21 +535,21 @@
         <v>7</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -561,19 +561,19 @@
         <v>5</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>